<commit_message>
XML Template fuer Benutzer und Lokalitaet angelegt , xml schema angepasst
</commit_message>
<xml_diff>
--- a/Kickercheck_Spezifikation.xlsx
+++ b/Kickercheck_Spezifikation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25823"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14660" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14680" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Blatt1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="131">
   <si>
     <t xml:space="preserve">Ressource </t>
   </si>
@@ -258,9 +258,6 @@
     <t>Löscht ein Turnier aus dem System , funktioniert nur als Ersteller des Tuniers. Turnier darf noch nicht gestartet sein</t>
   </si>
   <si>
-    <t xml:space="preserve">Bereitstellung einer Repräsentation einer Benutzressource , die über eine URI identifiziert ist </t>
-  </si>
-  <si>
     <t>/Kickertisch/{TischId}</t>
   </si>
   <si>
@@ -409,6 +406,12 @@
   </si>
   <si>
     <t>/Benutzer{id} oder /Benutzer{id}/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gleiche Dinge der realen Welt nur einmal im </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bereitstellung einer Repräsentation einer Benutzerressource </t>
   </si>
 </sst>
 </file>
@@ -480,8 +483,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="57">
+  <cellStyleXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -545,7 +556,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="57">
+  <cellStyles count="65">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
@@ -574,6 +585,10 @@
     <cellStyle name="Besuchter Link" xfId="52" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="54" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="64" builtinId="9" hidden="1"/>
     <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
@@ -602,6 +617,10 @@
     <cellStyle name="Link" xfId="51" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="53" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="63" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -931,10 +950,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H79"/>
+  <dimension ref="A1:H78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -972,7 +991,7 @@
         <v>50</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -983,16 +1002,16 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>79</v>
+        <v>130</v>
       </c>
       <c r="D2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E2" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="F2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G2" t="s">
         <v>52</v>
@@ -1009,13 +1028,13 @@
         <v>55</v>
       </c>
       <c r="D3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E3" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="F3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G3" t="s">
         <v>58</v>
@@ -1029,16 +1048,16 @@
         <v>54</v>
       </c>
       <c r="D4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E4" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="F4" t="s">
         <v>51</v>
       </c>
       <c r="G4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -1049,567 +1068,583 @@
         <v>56</v>
       </c>
       <c r="D5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F5" t="s">
         <v>51</v>
       </c>
       <c r="G5" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="20" customHeight="1">
-      <c r="A9" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="20" customHeight="1">
+      <c r="A8" t="s">
         <v>9</v>
       </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>57</v>
+      </c>
+      <c r="D8" t="s">
+        <v>92</v>
+      </c>
+      <c r="E8" t="s">
+        <v>100</v>
+      </c>
+      <c r="F8" t="s">
+        <v>63</v>
+      </c>
+      <c r="G8" t="s">
+        <v>52</v>
+      </c>
+      <c r="H8" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
       <c r="B9" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>57</v>
+        <v>101</v>
       </c>
       <c r="D9" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="E9" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="F9" t="s">
-        <v>63</v>
+        <v>108</v>
       </c>
       <c r="G9" t="s">
-        <v>52</v>
+        <v>106</v>
       </c>
       <c r="H9" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="B10" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C10" t="s">
-        <v>102</v>
+        <v>59</v>
       </c>
       <c r="D10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E10" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="F10" t="s">
+        <v>63</v>
+      </c>
+      <c r="G10" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" t="s">
+        <v>115</v>
+      </c>
+      <c r="B12" t="s">
+        <v>60</v>
+      </c>
+      <c r="C12" t="s">
+        <v>61</v>
+      </c>
+      <c r="D12" t="s">
+        <v>92</v>
+      </c>
+      <c r="E12" t="s">
+        <v>100</v>
+      </c>
+      <c r="F12" t="s">
+        <v>64</v>
+      </c>
+      <c r="G12" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="B13" t="s">
+        <v>62</v>
+      </c>
+      <c r="C13" t="s">
         <v>109</v>
       </c>
-      <c r="G10" t="s">
-        <v>107</v>
-      </c>
-      <c r="H10" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="B11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" t="s">
-        <v>59</v>
-      </c>
-      <c r="D11" t="s">
-        <v>90</v>
-      </c>
-      <c r="E11" t="s">
-        <v>101</v>
-      </c>
-      <c r="F11" t="s">
-        <v>63</v>
-      </c>
-      <c r="G11" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="A13" t="s">
-        <v>116</v>
-      </c>
-      <c r="B13" t="s">
-        <v>60</v>
-      </c>
-      <c r="C13" t="s">
-        <v>61</v>
-      </c>
       <c r="D13" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E13" t="s">
-        <v>101</v>
-      </c>
-      <c r="F13" t="s">
+        <v>100</v>
+      </c>
+      <c r="F13" s="3" t="s">
         <v>64</v>
       </c>
       <c r="G13" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
-      <c r="B14" t="s">
-        <v>62</v>
-      </c>
-      <c r="C14" t="s">
-        <v>110</v>
-      </c>
-      <c r="D14" t="s">
-        <v>93</v>
-      </c>
-      <c r="E14" t="s">
-        <v>101</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G14" t="s">
-        <v>112</v>
+    <row r="15" spans="1:8">
+      <c r="A15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" t="s">
+        <v>114</v>
+      </c>
+      <c r="D15" t="s">
+        <v>92</v>
+      </c>
+      <c r="E15" t="s">
+        <v>100</v>
+      </c>
+      <c r="F15" t="s">
+        <v>79</v>
+      </c>
+      <c r="G15" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" t="s">
-        <v>10</v>
-      </c>
       <c r="B16" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C16" t="s">
-        <v>115</v>
+        <v>123</v>
       </c>
       <c r="D16" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="E16" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="F16" t="s">
-        <v>80</v>
+        <v>117</v>
       </c>
       <c r="G16" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="17" spans="1:8">
       <c r="B17" t="s">
-        <v>6</v>
+        <v>62</v>
       </c>
       <c r="C17" t="s">
-        <v>124</v>
+        <v>65</v>
       </c>
       <c r="D17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E17" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="F17" t="s">
-        <v>118</v>
+        <v>79</v>
       </c>
       <c r="G17" t="s">
-        <v>125</v>
+        <v>104</v>
       </c>
     </row>
     <row r="18" spans="1:8">
       <c r="B18" t="s">
-        <v>62</v>
+        <v>8</v>
       </c>
       <c r="C18" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D18" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E18" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="F18" t="s">
+        <v>79</v>
+      </c>
+      <c r="G18" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" t="s">
+        <v>113</v>
+      </c>
+      <c r="B20" t="s">
+        <v>116</v>
+      </c>
+      <c r="C20" t="s">
+        <v>119</v>
+      </c>
+      <c r="D20" t="s">
+        <v>92</v>
+      </c>
+      <c r="E20" t="s">
+        <v>92</v>
+      </c>
+      <c r="F20" t="s">
+        <v>118</v>
+      </c>
+      <c r="G20" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="B21" t="s">
+        <v>70</v>
+      </c>
+      <c r="C21" t="s">
+        <v>121</v>
+      </c>
+      <c r="D21" t="s">
+        <v>92</v>
+      </c>
+      <c r="E21" t="s">
+        <v>92</v>
+      </c>
+      <c r="F21" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" t="s">
+        <v>66</v>
+      </c>
+      <c r="B23" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23" t="s">
+        <v>84</v>
+      </c>
+      <c r="D23" t="s">
+        <v>92</v>
+      </c>
+      <c r="E23" t="s">
+        <v>100</v>
+      </c>
+      <c r="F23" t="s">
         <v>80</v>
       </c>
-      <c r="G18" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8">
-      <c r="B19" t="s">
-        <v>8</v>
-      </c>
-      <c r="C19" t="s">
-        <v>67</v>
-      </c>
-      <c r="D19" t="s">
-        <v>93</v>
-      </c>
-      <c r="E19" t="s">
-        <v>93</v>
-      </c>
-      <c r="F19" t="s">
-        <v>80</v>
-      </c>
-      <c r="G19" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8">
-      <c r="A21" t="s">
-        <v>114</v>
-      </c>
-      <c r="B21" t="s">
-        <v>117</v>
-      </c>
-      <c r="C21" t="s">
-        <v>120</v>
-      </c>
-      <c r="D21" t="s">
-        <v>93</v>
-      </c>
-      <c r="E21" t="s">
-        <v>93</v>
-      </c>
-      <c r="F21" t="s">
-        <v>119</v>
-      </c>
-      <c r="G21" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8">
-      <c r="B22" t="s">
-        <v>70</v>
-      </c>
-      <c r="C22" t="s">
-        <v>122</v>
-      </c>
-      <c r="D22" t="s">
-        <v>93</v>
-      </c>
-      <c r="E22" t="s">
-        <v>93</v>
-      </c>
-      <c r="F22" t="s">
-        <v>123</v>
+      <c r="G23" t="s">
+        <v>52</v>
+      </c>
+      <c r="H23" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" t="s">
-        <v>66</v>
-      </c>
       <c r="B24" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C24" t="s">
-        <v>85</v>
+        <v>68</v>
       </c>
       <c r="D24" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="E24" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="F24" t="s">
-        <v>81</v>
+        <v>126</v>
       </c>
       <c r="G24" t="s">
-        <v>52</v>
-      </c>
-      <c r="H24" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
     </row>
     <row r="25" spans="1:8">
       <c r="B25" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C25" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D25" t="s">
-        <v>90</v>
+        <v>103</v>
       </c>
       <c r="E25" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="F25" t="s">
-        <v>127</v>
+        <v>80</v>
       </c>
       <c r="G25" t="s">
-        <v>58</v>
+        <v>104</v>
       </c>
     </row>
     <row r="26" spans="1:8">
       <c r="B26" t="s">
-        <v>7</v>
+        <v>70</v>
       </c>
       <c r="C26" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D26" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="E26" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="F26" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G26" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8">
-      <c r="B27" t="s">
-        <v>70</v>
-      </c>
-      <c r="C27" t="s">
-        <v>71</v>
-      </c>
-      <c r="D27" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" t="s">
+        <v>72</v>
+      </c>
+      <c r="B28" t="s">
+        <v>5</v>
+      </c>
+      <c r="C28" t="s">
+        <v>82</v>
+      </c>
+      <c r="D28" t="s">
+        <v>92</v>
+      </c>
+      <c r="E28" t="s">
+        <v>97</v>
+      </c>
+      <c r="F28" t="s">
+        <v>83</v>
+      </c>
+      <c r="G28" t="s">
+        <v>99</v>
+      </c>
+      <c r="H28" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="B29" t="s">
+        <v>6</v>
+      </c>
+      <c r="C29" t="s">
+        <v>73</v>
+      </c>
+      <c r="D29" t="s">
+        <v>89</v>
+      </c>
+      <c r="E29" t="s">
+        <v>91</v>
+      </c>
+      <c r="F29" t="s">
+        <v>83</v>
+      </c>
+      <c r="G29" t="s">
         <v>93</v>
       </c>
-      <c r="E27" t="s">
-        <v>93</v>
-      </c>
-      <c r="F27" t="s">
-        <v>81</v>
-      </c>
-      <c r="G27" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8">
-      <c r="A29" t="s">
-        <v>72</v>
-      </c>
-      <c r="B29" t="s">
-        <v>5</v>
-      </c>
-      <c r="C29" t="s">
-        <v>83</v>
-      </c>
-      <c r="D29" t="s">
-        <v>93</v>
-      </c>
-      <c r="E29" t="s">
-        <v>98</v>
-      </c>
-      <c r="F29" t="s">
-        <v>84</v>
-      </c>
-      <c r="G29" t="s">
-        <v>100</v>
-      </c>
       <c r="H29" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
     </row>
     <row r="30" spans="1:8">
       <c r="B30" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C30" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D30" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E30" t="s">
         <v>92</v>
       </c>
       <c r="F30" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G30" t="s">
         <v>94</v>
       </c>
       <c r="H30" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
     </row>
     <row r="31" spans="1:8">
       <c r="B31" t="s">
-        <v>7</v>
+        <v>70</v>
       </c>
       <c r="C31" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="D31" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E31" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F31" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G31" t="s">
         <v>95</v>
       </c>
-      <c r="H31" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8">
-      <c r="B32" t="s">
-        <v>70</v>
-      </c>
-      <c r="C32" t="s">
-        <v>82</v>
-      </c>
-      <c r="D32" t="s">
-        <v>93</v>
-      </c>
-      <c r="E32" t="s">
-        <v>93</v>
-      </c>
-      <c r="F32" t="s">
-        <v>84</v>
-      </c>
-      <c r="G32" t="s">
-        <v>96</v>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" t="s">
+        <v>75</v>
+      </c>
+      <c r="B33" t="s">
+        <v>5</v>
+      </c>
+      <c r="C33" t="s">
+        <v>76</v>
+      </c>
+      <c r="F33" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="34" spans="1:6">
-      <c r="A34" t="s">
-        <v>75</v>
-      </c>
       <c r="B34" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C34" t="s">
-        <v>76</v>
+        <v>127</v>
+      </c>
+      <c r="D34" t="s">
+        <v>89</v>
       </c>
       <c r="F34" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="35" spans="1:6">
       <c r="B35" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C35" t="s">
-        <v>128</v>
-      </c>
-      <c r="D35" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="F35" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="36" spans="1:6">
       <c r="B36" t="s">
-        <v>7</v>
+        <v>70</v>
       </c>
       <c r="C36" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F36" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="37" spans="1:6">
-      <c r="B37" t="s">
-        <v>70</v>
-      </c>
-      <c r="C37" t="s">
-        <v>78</v>
-      </c>
-      <c r="F37" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6">
-      <c r="A39" t="s">
+      <c r="B38" t="s">
+        <v>60</v>
+      </c>
+      <c r="C38" t="s">
+        <v>85</v>
+      </c>
+      <c r="F38" t="s">
         <v>88</v>
       </c>
-      <c r="B39" t="s">
-        <v>60</v>
-      </c>
-      <c r="C39" t="s">
-        <v>86</v>
-      </c>
-      <c r="F39" t="s">
-        <v>89</v>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="51" spans="1:4">
-      <c r="A51" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4">
-      <c r="A52" t="s">
+      <c r="A51" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="55" spans="1:4">
       <c r="A55" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4">
-      <c r="A56" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="A59" t="s">
+        <v>26</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="60" spans="1:4">
       <c r="A60" t="s">
-        <v>26</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>41</v>
+        <v>20</v>
+      </c>
+      <c r="C60" t="s">
+        <v>15</v>
+      </c>
+      <c r="D60" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="61" spans="1:4">
       <c r="A61" t="s">
-        <v>20</v>
-      </c>
-      <c r="C61" t="s">
-        <v>15</v>
-      </c>
-      <c r="D61" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="62" spans="1:4">
       <c r="A62" t="s">
-        <v>39</v>
+        <v>28</v>
+      </c>
+      <c r="C62" t="s">
+        <v>34</v>
+      </c>
+      <c r="D62" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="63" spans="1:4">
       <c r="A63" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="C63" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="D63" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="64" spans="1:4">
-      <c r="A64" t="s">
-        <v>45</v>
-      </c>
       <c r="C64" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D64" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="65" spans="1:4">
+      <c r="A65" t="s">
+        <v>33</v>
+      </c>
       <c r="C65" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="D65" t="s">
         <v>43</v>
@@ -1617,10 +1652,10 @@
     </row>
     <row r="66" spans="1:4">
       <c r="A66" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C66" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D66" t="s">
         <v>43</v>
@@ -1628,37 +1663,34 @@
     </row>
     <row r="67" spans="1:4">
       <c r="A67" t="s">
-        <v>29</v>
-      </c>
-      <c r="C67" t="s">
-        <v>37</v>
-      </c>
-      <c r="D67" t="s">
-        <v>43</v>
+        <v>21</v>
       </c>
     </row>
     <row r="68" spans="1:4">
       <c r="A68" t="s">
-        <v>21</v>
+        <v>30</v>
+      </c>
+      <c r="C68" t="s">
+        <v>18</v>
+      </c>
+      <c r="D68" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="69" spans="1:4">
       <c r="A69" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="C69" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D69" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="70" spans="1:4">
-      <c r="A70" t="s">
-        <v>11</v>
-      </c>
       <c r="C70" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="D70" t="s">
         <v>44</v>
@@ -1666,28 +1698,28 @@
     </row>
     <row r="71" spans="1:4">
       <c r="C71" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="D71" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="72" spans="1:4">
-      <c r="C72" t="s">
-        <v>25</v>
-      </c>
       <c r="D72" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="73" spans="1:4">
-      <c r="D73" t="s">
-        <v>44</v>
+    <row r="74" spans="1:4">
+      <c r="C74" t="s">
+        <v>27</v>
+      </c>
+      <c r="D74" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="75" spans="1:4">
       <c r="C75" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="D75" t="s">
         <v>46</v>
@@ -1695,30 +1727,22 @@
     </row>
     <row r="76" spans="1:4">
       <c r="C76" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D76" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="77" spans="1:4">
       <c r="C77" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D77" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="78" spans="1:4">
       <c r="C78" t="s">
-        <v>31</v>
-      </c>
-      <c r="D78" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4">
-      <c r="C79" t="s">
         <v>40</v>
       </c>
     </row>

</xml_diff>